<commit_message>
Code Refinement, Error Handling, UI Enhancement
</commit_message>
<xml_diff>
--- a/topic_ids_v3.xlsx
+++ b/topic_ids_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darshan/Code/capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8755CE13-DE24-054F-AC02-D429C09C4610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17829505-BA54-674D-AD8C-EFF5FA71135E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="1140" windowWidth="27240" windowHeight="16440" xr2:uid="{D9440E26-C594-174E-9B63-878DC898CA49}"/>
+    <workbookView xWindow="5800" yWindow="3560" windowWidth="27240" windowHeight="16440" xr2:uid="{D9440E26-C594-174E-9B63-878DC898CA49}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_ids" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>key_name</t>
   </si>
@@ -176,9 +176,6 @@
     <t xml:space="preserve">Mathematics for Data Science </t>
   </si>
   <si>
-    <t>Excel</t>
-  </si>
-  <si>
     <t>Data Minning</t>
   </si>
   <si>
@@ -189,6 +186,72 @@
   </si>
   <si>
     <t xml:space="preserve">LangChain Library </t>
+  </si>
+  <si>
+    <t>Heat map</t>
+  </si>
+  <si>
+    <t>Violin plot</t>
+  </si>
+  <si>
+    <t>Swarm plot</t>
+  </si>
+  <si>
+    <t>Facet grid</t>
+  </si>
+  <si>
+    <t>Loading datasets</t>
+  </si>
+  <si>
+    <t>Installing seaborn</t>
+  </si>
+  <si>
+    <t>scatter plot</t>
+  </si>
+  <si>
+    <t>line plot</t>
+  </si>
+  <si>
+    <t>Histogram</t>
+  </si>
+  <si>
+    <t>box plot</t>
+  </si>
+  <si>
+    <t>pairplot</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbors</t>
+  </si>
+  <si>
+    <t>Decision trees</t>
+  </si>
+  <si>
+    <t>Bayesian</t>
+  </si>
+  <si>
+    <t>Kernel Methods</t>
+  </si>
+  <si>
+    <t>Clustering Methods</t>
+  </si>
+  <si>
+    <t>Estimator API</t>
+  </si>
+  <si>
+    <t>pytorch</t>
+  </si>
+  <si>
+    <t>Keras</t>
+  </si>
+  <si>
+    <t>Big Data Analytics</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Language Models </t>
   </si>
 </sst>
 </file>
@@ -580,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530F23A1-6A55-404B-B7DD-1CA37AED3A54}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,7 +1018,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -963,7 +1026,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -971,7 +1034,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -979,7 +1042,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -987,92 +1050,176 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>51</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>52</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>53</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>54</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>55</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>56</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>57</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>58</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>59</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>60</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>61</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>62</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>63</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>64</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>65</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>66</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>67</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>68</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>69</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>70</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>71</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>

</xml_diff>